<commit_message>
Tiny update - starting page
</commit_message>
<xml_diff>
--- a/SquareCity.xlsx
+++ b/SquareCity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RawBefore" sheetId="1" r:id="rId1"/>
@@ -437,16 +437,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -457,26 +449,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,17 +472,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="16">
     <dxf>
       <font>
         <color theme="4" tint="-0.24994659260841701"/>
@@ -592,228 +592,6 @@
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -1310,7 +1088,7 @@
       <c r="AI1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="50" t="s">
+      <c r="AJ1" s="40" t="s">
         <v>1</v>
       </c>
       <c r="AK1">
@@ -1427,7 +1205,7 @@
       <c r="AI2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ2" s="50" t="s">
+      <c r="AJ2" s="40" t="s">
         <v>1</v>
       </c>
       <c r="AK2">
@@ -1544,7 +1322,7 @@
       <c r="AI3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ3" s="50" t="s">
+      <c r="AJ3" s="40" t="s">
         <v>1</v>
       </c>
       <c r="AK3">
@@ -1661,10 +1439,10 @@
       <c r="AI4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ4" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="30">
+      <c r="AJ4" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="28">
         <f>+AK2/AK3</f>
         <v>0.54861111111111116</v>
       </c>
@@ -1778,7 +1556,7 @@
       <c r="AI5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="50" t="s">
+      <c r="AJ5" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1888,7 +1666,7 @@
       <c r="AI6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ6" s="51" t="s">
+      <c r="AJ6" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1998,7 +1776,7 @@
       <c r="AI7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ7" s="50" t="s">
+      <c r="AJ7" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2108,7 +1886,7 @@
       <c r="AI8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ8" s="51" t="s">
+      <c r="AJ8" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2218,7 +1996,7 @@
       <c r="AI9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ9" s="50" t="s">
+      <c r="AJ9" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2328,7 +2106,7 @@
       <c r="AI10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ10" s="51" t="s">
+      <c r="AJ10" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2438,7 +2216,7 @@
       <c r="AI11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ11" s="50" t="s">
+      <c r="AJ11" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2548,7 +2326,7 @@
       <c r="AI12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ12" s="51" t="s">
+      <c r="AJ12" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2658,7 +2436,7 @@
       <c r="AI13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ13" s="50" t="s">
+      <c r="AJ13" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2768,7 +2546,7 @@
       <c r="AI14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ14" s="51" t="s">
+      <c r="AJ14" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2878,7 +2656,7 @@
       <c r="AI15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ15" s="50" t="s">
+      <c r="AJ15" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2988,7 +2766,7 @@
       <c r="AI16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ16" s="51" t="s">
+      <c r="AJ16" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3098,7 +2876,7 @@
       <c r="AI17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ17" s="50" t="s">
+      <c r="AJ17" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3208,7 +2986,7 @@
       <c r="AI18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ18" s="51" t="s">
+      <c r="AJ18" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3318,7 +3096,7 @@
       <c r="AI19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ19" s="50" t="s">
+      <c r="AJ19" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3428,7 +3206,7 @@
       <c r="AI20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ20" s="51" t="s">
+      <c r="AJ20" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3538,7 +3316,7 @@
       <c r="AI21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ21" s="50" t="s">
+      <c r="AJ21" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3648,7 +3426,7 @@
       <c r="AI22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ22" s="51" t="s">
+      <c r="AJ22" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3758,7 +3536,7 @@
       <c r="AI23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ23" s="50" t="s">
+      <c r="AJ23" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3868,7 +3646,7 @@
       <c r="AI24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ24" s="50" t="s">
+      <c r="AJ24" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3978,7 +3756,7 @@
       <c r="AI25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ25" s="50" t="s">
+      <c r="AJ25" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4088,7 +3866,7 @@
       <c r="AI26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ26" s="51" t="s">
+      <c r="AJ26" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4198,7 +3976,7 @@
       <c r="AI27" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ27" s="50" t="s">
+      <c r="AJ27" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4308,7 +4086,7 @@
       <c r="AI28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ28" s="51" t="s">
+      <c r="AJ28" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4418,7 +4196,7 @@
       <c r="AI29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ29" s="50" t="s">
+      <c r="AJ29" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4528,7 +4306,7 @@
       <c r="AI30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ30" s="51" t="s">
+      <c r="AJ30" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4638,7 +4416,7 @@
       <c r="AI31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ31" s="50" t="s">
+      <c r="AJ31" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4748,7 +4526,7 @@
       <c r="AI32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ32" s="51" t="s">
+      <c r="AJ32" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4858,7 +4636,7 @@
       <c r="AI33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ33" s="50" t="s">
+      <c r="AJ33" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4968,7 +4746,7 @@
       <c r="AI34" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ34" s="51" t="s">
+      <c r="AJ34" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5078,7 +4856,7 @@
       <c r="AI35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ35" s="50" t="s">
+      <c r="AJ35" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5188,7 +4966,7 @@
       <c r="AI36" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AJ36" s="51" t="s">
+      <c r="AJ36" s="41" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5322,7 +5100,7 @@
       <c r="AI1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ1" s="52" t="s">
+      <c r="AJ1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK1">
@@ -5439,7 +5217,7 @@
       <c r="AI2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ2" s="52" t="s">
+      <c r="AJ2" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK2">
@@ -5556,7 +5334,7 @@
       <c r="AI3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ3" s="52" t="s">
+      <c r="AJ3" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK3">
@@ -5673,10 +5451,10 @@
       <c r="AI4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ4" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="30">
+      <c r="AJ4" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="28">
         <f>+AK2/AK3</f>
         <v>0.49305555555555558</v>
       </c>
@@ -5790,7 +5568,7 @@
       <c r="AI5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ5" s="52" t="s">
+      <c r="AJ5" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK5" s="7"/>
@@ -5901,7 +5679,7 @@
       <c r="AI6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ6" s="53" t="s">
+      <c r="AJ6" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK6" s="7"/>
@@ -6012,7 +5790,7 @@
       <c r="AI7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ7" s="52" t="s">
+      <c r="AJ7" s="42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6122,7 +5900,7 @@
       <c r="AI8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ8" s="53" t="s">
+      <c r="AJ8" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK8" s="7"/>
@@ -6233,7 +6011,7 @@
       <c r="AI9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ9" s="52" t="s">
+      <c r="AJ9" s="42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6343,7 +6121,7 @@
       <c r="AI10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ10" s="53" t="s">
+      <c r="AJ10" s="43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6453,7 +6231,7 @@
       <c r="AI11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ11" s="52" t="s">
+      <c r="AJ11" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK11" s="7"/>
@@ -6564,7 +6342,7 @@
       <c r="AI12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ12" s="53" t="s">
+      <c r="AJ12" s="43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6674,7 +6452,7 @@
       <c r="AI13" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ13" s="52" t="s">
+      <c r="AJ13" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK13" s="7"/>
@@ -6785,7 +6563,7 @@
       <c r="AI14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ14" s="53" t="s">
+      <c r="AJ14" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK14" s="7"/>
@@ -6896,7 +6674,7 @@
       <c r="AI15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ15" s="52" t="s">
+      <c r="AJ15" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK15" s="7"/>
@@ -7007,7 +6785,7 @@
       <c r="AI16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ16" s="53" t="s">
+      <c r="AJ16" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK16" s="7"/>
@@ -7118,7 +6896,7 @@
       <c r="AI17" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ17" s="53" t="s">
+      <c r="AJ17" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK17" s="7"/>
@@ -7229,7 +7007,7 @@
       <c r="AI18" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ18" s="53" t="s">
+      <c r="AJ18" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK18" s="7"/>
@@ -7340,7 +7118,7 @@
       <c r="AI19" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ19" s="52" t="s">
+      <c r="AJ19" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK19" s="7"/>
@@ -7451,7 +7229,7 @@
       <c r="AI20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ20" s="53" t="s">
+      <c r="AJ20" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK20" s="7"/>
@@ -7562,7 +7340,7 @@
       <c r="AI21" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ21" s="52" t="s">
+      <c r="AJ21" s="42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7672,7 +7450,7 @@
       <c r="AI22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ22" s="53" t="s">
+      <c r="AJ22" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK22" s="7"/>
@@ -7783,7 +7561,7 @@
       <c r="AI23" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ23" s="52" t="s">
+      <c r="AJ23" s="42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -7893,7 +7671,7 @@
       <c r="AI24" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ24" s="52" t="s">
+      <c r="AJ24" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK24" s="7"/>
@@ -8004,7 +7782,7 @@
       <c r="AI25" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ25" s="52" t="s">
+      <c r="AJ25" s="42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8114,7 +7892,7 @@
       <c r="AI26" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ26" s="53" t="s">
+      <c r="AJ26" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK26" s="7"/>
@@ -8225,7 +8003,7 @@
       <c r="AI27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ27" s="52" t="s">
+      <c r="AJ27" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK27" s="7"/>
@@ -8336,7 +8114,7 @@
       <c r="AI28" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ28" s="53" t="s">
+      <c r="AJ28" s="43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8446,7 +8224,7 @@
       <c r="AI29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ29" s="52" t="s">
+      <c r="AJ29" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK29" s="7"/>
@@ -8557,7 +8335,7 @@
       <c r="AI30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ30" s="53" t="s">
+      <c r="AJ30" s="43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -8667,7 +8445,7 @@
       <c r="AI31" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ31" s="52" t="s">
+      <c r="AJ31" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK31" s="7"/>
@@ -8778,7 +8556,7 @@
       <c r="AI32" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ32" s="53" t="s">
+      <c r="AJ32" s="43" t="s">
         <v>0</v>
       </c>
       <c r="AK32" s="7"/>
@@ -8889,7 +8667,7 @@
       <c r="AI33" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ33" s="52" t="s">
+      <c r="AJ33" s="42" t="s">
         <v>1</v>
       </c>
       <c r="AK33" s="7"/>
@@ -9000,7 +8778,7 @@
       <c r="AI34" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ34" s="53" t="s">
+      <c r="AJ34" s="43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9110,7 +8888,7 @@
       <c r="AI35" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="AJ35" s="52" t="s">
+      <c r="AJ35" s="42" t="s">
         <v>1</v>
       </c>
     </row>
@@ -9220,7 +8998,7 @@
       <c r="AI36" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AJ36" s="53" t="s">
+      <c r="AJ36" s="43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9459,7 +9237,7 @@
         <f>(IF(RawBefore!AI1 = RawAfter!AI1, " ", RawAfter!AI1))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ1" s="53" t="str">
+      <c r="AJ1" s="43" t="str">
         <f>(IF(RawBefore!AJ1 = RawAfter!AJ1, " ", RawAfter!AJ1))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -9612,7 +9390,7 @@
         <f>(IF(RawBefore!AI2 = RawAfter!AI2, " ", RawAfter!AI2))</f>
         <v>B</v>
       </c>
-      <c r="AJ2" s="53" t="str">
+      <c r="AJ2" s="43" t="str">
         <f>(IF(RawBefore!AJ2 = RawAfter!AJ2, " ", RawAfter!AJ2))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -9765,7 +9543,7 @@
         <f>(IF(RawBefore!AI3 = RawAfter!AI3, " ", RawAfter!AI3))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ3" s="53" t="str">
+      <c r="AJ3" s="43" t="str">
         <f>(IF(RawBefore!AJ3 = RawAfter!AJ3, " ", RawAfter!AJ3))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -9911,7 +9689,7 @@
         <f>(IF(RawBefore!AI4 = RawAfter!AI4, " ", RawAfter!AI4))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ4" s="53" t="str">
+      <c r="AJ4" s="43" t="str">
         <f>(IF(RawBefore!AJ4 = RawAfter!AJ4, " ", RawAfter!AJ4))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10064,7 +9842,7 @@
         <f>(IF(RawBefore!AI5 = RawAfter!AI5, " ", RawAfter!AI5))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ5" s="53" t="str">
+      <c r="AJ5" s="43" t="str">
         <f>(IF(RawBefore!AJ5 = RawAfter!AJ5, " ", RawAfter!AJ5))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10217,7 +9995,7 @@
         <f>(IF(RawBefore!AI6 = RawAfter!AI6, " ", RawAfter!AI6))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ6" s="53" t="str">
+      <c r="AJ6" s="43" t="str">
         <f>(IF(RawBefore!AJ6 = RawAfter!AJ6, " ", RawAfter!AJ6))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10364,7 +10142,7 @@
         <f>(IF(RawBefore!AI7 = RawAfter!AI7, " ", RawAfter!AI7))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ7" s="53" t="str">
+      <c r="AJ7" s="43" t="str">
         <f>(IF(RawBefore!AJ7 = RawAfter!AJ7, " ", RawAfter!AJ7))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10517,7 +10295,7 @@
         <f>(IF(RawBefore!AI8 = RawAfter!AI8, " ", RawAfter!AI8))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ8" s="53" t="str">
+      <c r="AJ8" s="43" t="str">
         <f>(IF(RawBefore!AJ8 = RawAfter!AJ8, " ", RawAfter!AJ8))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10663,7 +10441,7 @@
         <f>(IF(RawBefore!AI9 = RawAfter!AI9, " ", RawAfter!AI9))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ9" s="53" t="str">
+      <c r="AJ9" s="43" t="str">
         <f>(IF(RawBefore!AJ9 = RawAfter!AJ9, " ", RawAfter!AJ9))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -10816,11 +10594,11 @@
         <f>(IF(RawBefore!AI10 = RawAfter!AI10, " ", RawAfter!AI10))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ10" s="53" t="str">
+      <c r="AJ10" s="43" t="str">
         <f>(IF(RawBefore!AJ10 = RawAfter!AJ10, " ", RawAfter!AJ10))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AK10" s="29">
+      <c r="AK10" s="27">
         <f>+AK9/AK7</f>
         <v>5.5555555555555552E-2</v>
       </c>
@@ -10969,7 +10747,7 @@
         <f>(IF(RawBefore!AI11 = RawAfter!AI11, " ", RawAfter!AI11))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ11" s="53" t="str">
+      <c r="AJ11" s="43" t="str">
         <f>(IF(RawBefore!AJ11 = RawAfter!AJ11, " ", RawAfter!AJ11))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -11115,7 +10893,7 @@
         <f>(IF(RawBefore!AI12 = RawAfter!AI12, " ", RawAfter!AI12))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ12" s="53" t="str">
+      <c r="AJ12" s="43" t="str">
         <f>(IF(RawBefore!AJ12 = RawAfter!AJ12, " ", RawAfter!AJ12))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -11261,7 +11039,7 @@
         <f>(IF(RawBefore!AI13 = RawAfter!AI13, " ", RawAfter!AI13))</f>
         <v>B</v>
       </c>
-      <c r="AJ13" s="53" t="str">
+      <c r="AJ13" s="43" t="str">
         <f>(IF(RawBefore!AJ13 = RawAfter!AJ13, " ", RawAfter!AJ13))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -11407,7 +11185,7 @@
         <f>(IF(RawBefore!AI14 = RawAfter!AI14, " ", RawAfter!AI14))</f>
         <v>B</v>
       </c>
-      <c r="AJ14" s="53" t="str">
+      <c r="AJ14" s="43" t="str">
         <f>(IF(RawBefore!AJ14 = RawAfter!AJ14, " ", RawAfter!AJ14))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -11554,7 +11332,7 @@
         <f>(IF(RawBefore!AI15 = RawAfter!AI15, " ", RawAfter!AI15))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ15" s="53" t="str">
+      <c r="AJ15" s="43" t="str">
         <f>(IF(RawBefore!AJ15 = RawAfter!AJ15, " ", RawAfter!AJ15))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -11701,7 +11479,7 @@
         <f>(IF(RawBefore!AI16 = RawAfter!AI16, " ", RawAfter!AI16))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ16" s="53" t="str">
+      <c r="AJ16" s="43" t="str">
         <f>(IF(RawBefore!AJ16 = RawAfter!AJ16, " ", RawAfter!AJ16))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -11847,7 +11625,7 @@
         <f>(IF(RawBefore!AI17 = RawAfter!AI17, " ", RawAfter!AI17))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ17" s="53" t="str">
+      <c r="AJ17" s="43" t="str">
         <f>(IF(RawBefore!AJ17 = RawAfter!AJ17, " ", RawAfter!AJ17))</f>
         <v>B</v>
       </c>
@@ -11993,7 +11771,7 @@
         <f>(IF(RawBefore!AI18 = RawAfter!AI18, " ", RawAfter!AI18))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ18" s="53" t="str">
+      <c r="AJ18" s="43" t="str">
         <f>(IF(RawBefore!AJ18 = RawAfter!AJ18, " ", RawAfter!AJ18))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -12139,7 +11917,7 @@
         <f>(IF(RawBefore!AI19 = RawAfter!AI19, " ", RawAfter!AI19))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ19" s="53" t="str">
+      <c r="AJ19" s="43" t="str">
         <f>(IF(RawBefore!AJ19 = RawAfter!AJ19, " ", RawAfter!AJ19))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -12286,7 +12064,7 @@
         <f>(IF(RawBefore!AI20 = RawAfter!AI20, " ", RawAfter!AI20))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ20" s="53" t="str">
+      <c r="AJ20" s="43" t="str">
         <f>(IF(RawBefore!AJ20 = RawAfter!AJ20, " ", RawAfter!AJ20))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -12433,7 +12211,7 @@
         <f>(IF(RawBefore!AI21 = RawAfter!AI21, " ", RawAfter!AI21))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ21" s="53" t="str">
+      <c r="AJ21" s="43" t="str">
         <f>(IF(RawBefore!AJ21 = RawAfter!AJ21, " ", RawAfter!AJ21))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -12579,7 +12357,7 @@
         <f>(IF(RawBefore!AI22 = RawAfter!AI22, " ", RawAfter!AI22))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ22" s="53" t="str">
+      <c r="AJ22" s="43" t="str">
         <f>(IF(RawBefore!AJ22 = RawAfter!AJ22, " ", RawAfter!AJ22))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -12726,7 +12504,7 @@
         <f>(IF(RawBefore!AI23 = RawAfter!AI23, " ", RawAfter!AI23))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ23" s="53" t="str">
+      <c r="AJ23" s="43" t="str">
         <f>(IF(RawBefore!AJ23 = RawAfter!AJ23, " ", RawAfter!AJ23))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -12872,7 +12650,7 @@
         <f>(IF(RawBefore!AI24 = RawAfter!AI24, " ", RawAfter!AI24))</f>
         <v>B</v>
       </c>
-      <c r="AJ24" s="53" t="str">
+      <c r="AJ24" s="43" t="str">
         <f>(IF(RawBefore!AJ24 = RawAfter!AJ24, " ", RawAfter!AJ24))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13019,7 +12797,7 @@
         <f>(IF(RawBefore!AI25 = RawAfter!AI25, " ", RawAfter!AI25))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ25" s="53" t="str">
+      <c r="AJ25" s="43" t="str">
         <f>(IF(RawBefore!AJ25 = RawAfter!AJ25, " ", RawAfter!AJ25))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13165,7 +12943,7 @@
         <f>(IF(RawBefore!AI26 = RawAfter!AI26, " ", RawAfter!AI26))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ26" s="53" t="str">
+      <c r="AJ26" s="43" t="str">
         <f>(IF(RawBefore!AJ26 = RawAfter!AJ26, " ", RawAfter!AJ26))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13312,7 +13090,7 @@
         <f>(IF(RawBefore!AI27 = RawAfter!AI27, " ", RawAfter!AI27))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ27" s="53" t="str">
+      <c r="AJ27" s="43" t="str">
         <f>(IF(RawBefore!AJ27 = RawAfter!AJ27, " ", RawAfter!AJ27))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13459,7 +13237,7 @@
         <f>(IF(RawBefore!AI28 = RawAfter!AI28, " ", RawAfter!AI28))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ28" s="53" t="str">
+      <c r="AJ28" s="43" t="str">
         <f>(IF(RawBefore!AJ28 = RawAfter!AJ28, " ", RawAfter!AJ28))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13605,7 +13383,7 @@
         <f>(IF(RawBefore!AI29 = RawAfter!AI29, " ", RawAfter!AI29))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ29" s="53" t="str">
+      <c r="AJ29" s="43" t="str">
         <f>(IF(RawBefore!AJ29 = RawAfter!AJ29, " ", RawAfter!AJ29))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13752,7 +13530,7 @@
         <f>(IF(RawBefore!AI30 = RawAfter!AI30, " ", RawAfter!AI30))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ30" s="53" t="str">
+      <c r="AJ30" s="43" t="str">
         <f>(IF(RawBefore!AJ30 = RawAfter!AJ30, " ", RawAfter!AJ30))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -13898,7 +13676,7 @@
         <f>(IF(RawBefore!AI31 = RawAfter!AI31, " ", RawAfter!AI31))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ31" s="53" t="str">
+      <c r="AJ31" s="43" t="str">
         <f>(IF(RawBefore!AJ31 = RawAfter!AJ31, " ", RawAfter!AJ31))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -14045,7 +13823,7 @@
         <f>(IF(RawBefore!AI32 = RawAfter!AI32, " ", RawAfter!AI32))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ32" s="53" t="str">
+      <c r="AJ32" s="43" t="str">
         <f>(IF(RawBefore!AJ32 = RawAfter!AJ32, " ", RawAfter!AJ32))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -14192,7 +13970,7 @@
         <f>(IF(RawBefore!AI33 = RawAfter!AI33, " ", RawAfter!AI33))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ33" s="53" t="str">
+      <c r="AJ33" s="43" t="str">
         <f>(IF(RawBefore!AJ33 = RawAfter!AJ33, " ", RawAfter!AJ33))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -14339,7 +14117,7 @@
         <f>(IF(RawBefore!AI34 = RawAfter!AI34, " ", RawAfter!AI34))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ34" s="53" t="str">
+      <c r="AJ34" s="43" t="str">
         <f>(IF(RawBefore!AJ34 = RawAfter!AJ34, " ", RawAfter!AJ34))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -14485,7 +14263,7 @@
         <f>(IF(RawBefore!AI35 = RawAfter!AI35, " ", RawAfter!AI35))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ35" s="53" t="str">
+      <c r="AJ35" s="43" t="str">
         <f>(IF(RawBefore!AJ35 = RawAfter!AJ35, " ", RawAfter!AJ35))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -14631,7 +14409,7 @@
         <f>(IF(RawBefore!AI36 = RawAfter!AI36, " ", RawAfter!AI36))</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="AJ36" s="53" t="str">
+      <c r="AJ36" s="43" t="str">
         <f>(IF(RawBefore!AJ36 = RawAfter!AJ36, " ", RawAfter!AJ36))</f>
         <v xml:space="preserve"> </v>
       </c>
@@ -14718,7 +14496,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AS36"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="AL23" sqref="AL23"/>
     </sheetView>
   </sheetViews>
@@ -15523,7 +15301,7 @@
         <f>+RawBefore!AJ5</f>
         <v>R</v>
       </c>
-      <c r="AL5" s="35" t="s">
+      <c r="AL5" s="31" t="s">
         <v>9</v>
       </c>
       <c r="AM5" s="19">
@@ -15830,21 +15608,21 @@
         <f>+RawBefore!AJ7</f>
         <v>R</v>
       </c>
-      <c r="AL7" s="31" t="str">
+      <c r="AL7" s="44" t="str">
         <f>IF(AM5&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AM7" s="32"/>
-      <c r="AO7" s="31" t="str">
+      <c r="AM7" s="45"/>
+      <c r="AO7" s="44" t="str">
         <f>IF(AP5&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AP7" s="32"/>
-      <c r="AR7" s="31" t="str">
+      <c r="AP7" s="45"/>
+      <c r="AR7" s="44" t="str">
         <f>IF(AS5&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AS7" s="32"/>
+      <c r="AS7" s="45"/>
     </row>
     <row r="8" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="str">
@@ -15991,12 +15769,12 @@
         <f>+RawBefore!AJ8</f>
         <v>B</v>
       </c>
-      <c r="AL8" s="32"/>
-      <c r="AM8" s="32"/>
-      <c r="AO8" s="32"/>
-      <c r="AP8" s="32"/>
-      <c r="AR8" s="32"/>
-      <c r="AS8" s="32"/>
+      <c r="AL8" s="45"/>
+      <c r="AM8" s="45"/>
+      <c r="AO8" s="45"/>
+      <c r="AP8" s="45"/>
+      <c r="AR8" s="45"/>
+      <c r="AS8" s="45"/>
     </row>
     <row r="9" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="str">
@@ -17374,7 +17152,7 @@
         <f>+RawBefore!AJ17</f>
         <v>R</v>
       </c>
-      <c r="AL17" s="35" t="s">
+      <c r="AL17" s="31" t="s">
         <v>9</v>
       </c>
       <c r="AM17" s="19">
@@ -17681,21 +17459,21 @@
         <f>+RawBefore!AJ19</f>
         <v>R</v>
       </c>
-      <c r="AL19" s="31" t="str">
+      <c r="AL19" s="44" t="str">
         <f>IF(AM17&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AM19" s="32"/>
-      <c r="AO19" s="31" t="str">
+      <c r="AM19" s="45"/>
+      <c r="AO19" s="44" t="str">
         <f>IF(AP17&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AP19" s="32"/>
-      <c r="AR19" s="31" t="str">
+      <c r="AP19" s="45"/>
+      <c r="AR19" s="44" t="str">
         <f>IF(AS17&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AS19" s="32"/>
+      <c r="AS19" s="45"/>
     </row>
     <row r="20" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="str">
@@ -17842,12 +17620,12 @@
         <f>+RawBefore!AJ20</f>
         <v>B</v>
       </c>
-      <c r="AL20" s="32"/>
-      <c r="AM20" s="32"/>
-      <c r="AO20" s="32"/>
-      <c r="AP20" s="32"/>
-      <c r="AR20" s="32"/>
-      <c r="AS20" s="32"/>
+      <c r="AL20" s="45"/>
+      <c r="AM20" s="45"/>
+      <c r="AO20" s="45"/>
+      <c r="AP20" s="45"/>
+      <c r="AR20" s="45"/>
+      <c r="AS20" s="45"/>
     </row>
     <row r="21" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="str">
@@ -19225,7 +19003,7 @@
         <f>+RawBefore!AJ29</f>
         <v>R</v>
       </c>
-      <c r="AL29" s="35" t="s">
+      <c r="AL29" s="31" t="s">
         <v>9</v>
       </c>
       <c r="AM29" s="19">
@@ -19532,21 +19310,21 @@
         <f>+RawBefore!AJ31</f>
         <v>R</v>
       </c>
-      <c r="AL31" s="31" t="str">
+      <c r="AL31" s="44" t="str">
         <f>IF(AM29&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AM31" s="32"/>
-      <c r="AO31" s="31" t="str">
+      <c r="AM31" s="45"/>
+      <c r="AO31" s="44" t="str">
         <f>IF(AP29&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AP31" s="32"/>
-      <c r="AR31" s="31" t="str">
+      <c r="AP31" s="45"/>
+      <c r="AR31" s="44" t="str">
         <f>IF(AS29&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AS31" s="32"/>
+      <c r="AS31" s="45"/>
     </row>
     <row r="32" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="str">
@@ -19693,12 +19471,12 @@
         <f>+RawBefore!AJ32</f>
         <v>B</v>
       </c>
-      <c r="AL32" s="32"/>
-      <c r="AM32" s="32"/>
-      <c r="AO32" s="32"/>
-      <c r="AP32" s="32"/>
-      <c r="AR32" s="32"/>
-      <c r="AS32" s="32"/>
+      <c r="AL32" s="45"/>
+      <c r="AM32" s="45"/>
+      <c r="AO32" s="45"/>
+      <c r="AP32" s="45"/>
+      <c r="AR32" s="45"/>
+      <c r="AS32" s="45"/>
     </row>
     <row r="33" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="str">
@@ -21129,7 +20907,7 @@
         <f>+RawAfter!AJ5</f>
         <v>R</v>
       </c>
-      <c r="AL5" s="35" t="s">
+      <c r="AL5" s="31" t="s">
         <v>9</v>
       </c>
       <c r="AM5" s="19">
@@ -21436,21 +21214,21 @@
         <f>+RawAfter!AJ7</f>
         <v>R</v>
       </c>
-      <c r="AL7" s="31" t="str">
+      <c r="AL7" s="44" t="str">
         <f>IF(AM5&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AM7" s="32"/>
-      <c r="AO7" s="31" t="str">
+      <c r="AM7" s="45"/>
+      <c r="AO7" s="44" t="str">
         <f>IF(AP5&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AP7" s="32"/>
-      <c r="AR7" s="31" t="str">
+      <c r="AP7" s="45"/>
+      <c r="AR7" s="44" t="str">
         <f>IF(AS5&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AS7" s="32"/>
+      <c r="AS7" s="45"/>
     </row>
     <row r="8" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
@@ -21597,12 +21375,12 @@
         <f>+RawAfter!AJ8</f>
         <v>B</v>
       </c>
-      <c r="AL8" s="32"/>
-      <c r="AM8" s="32"/>
-      <c r="AO8" s="32"/>
-      <c r="AP8" s="32"/>
-      <c r="AR8" s="32"/>
-      <c r="AS8" s="32"/>
+      <c r="AL8" s="45"/>
+      <c r="AM8" s="45"/>
+      <c r="AO8" s="45"/>
+      <c r="AP8" s="45"/>
+      <c r="AR8" s="45"/>
+      <c r="AS8" s="45"/>
     </row>
     <row r="9" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
@@ -22980,7 +22758,7 @@
         <f>+RawAfter!AJ17</f>
         <v>B</v>
       </c>
-      <c r="AL17" s="35" t="s">
+      <c r="AL17" s="31" t="s">
         <v>9</v>
       </c>
       <c r="AM17" s="19">
@@ -23287,21 +23065,21 @@
         <f>+RawAfter!AJ19</f>
         <v>R</v>
       </c>
-      <c r="AL19" s="31" t="str">
+      <c r="AL19" s="44" t="str">
         <f>IF(AM17&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AM19" s="32"/>
-      <c r="AO19" s="31" t="str">
+      <c r="AM19" s="45"/>
+      <c r="AO19" s="44" t="str">
         <f>IF(AP17&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AP19" s="32"/>
-      <c r="AR19" s="31" t="str">
+      <c r="AP19" s="45"/>
+      <c r="AR19" s="44" t="str">
         <f>IF(AS17&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AS19" s="32"/>
+      <c r="AS19" s="45"/>
     </row>
     <row r="20" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
@@ -23448,12 +23226,12 @@
         <f>+RawAfter!AJ20</f>
         <v>B</v>
       </c>
-      <c r="AL20" s="32"/>
-      <c r="AM20" s="32"/>
-      <c r="AO20" s="32"/>
-      <c r="AP20" s="32"/>
-      <c r="AR20" s="32"/>
-      <c r="AS20" s="32"/>
+      <c r="AL20" s="45"/>
+      <c r="AM20" s="45"/>
+      <c r="AO20" s="45"/>
+      <c r="AP20" s="45"/>
+      <c r="AR20" s="45"/>
+      <c r="AS20" s="45"/>
     </row>
     <row r="21" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
@@ -24831,7 +24609,7 @@
         <f>+RawAfter!AJ29</f>
         <v>R</v>
       </c>
-      <c r="AL29" s="35" t="s">
+      <c r="AL29" s="31" t="s">
         <v>9</v>
       </c>
       <c r="AM29" s="19">
@@ -25138,21 +24916,21 @@
         <f>+RawAfter!AJ31</f>
         <v>R</v>
       </c>
-      <c r="AL31" s="31" t="str">
+      <c r="AL31" s="44" t="str">
         <f>IF(AM29&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AM31" s="32"/>
-      <c r="AO31" s="31" t="str">
+      <c r="AM31" s="45"/>
+      <c r="AO31" s="44" t="str">
         <f>IF(AP29&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AP31" s="32"/>
-      <c r="AR31" s="31" t="str">
+      <c r="AP31" s="45"/>
+      <c r="AR31" s="44" t="str">
         <f>IF(AS29&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AS31" s="32"/>
+      <c r="AS31" s="45"/>
     </row>
     <row r="32" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
@@ -25171,7 +24949,7 @@
         <f>+RawAfter!D32</f>
         <v>B</v>
       </c>
-      <c r="E32" s="49" t="str">
+      <c r="E32" s="39" t="str">
         <f>+RawAfter!E32</f>
         <v>R</v>
       </c>
@@ -25299,12 +25077,12 @@
         <f>+RawAfter!AJ32</f>
         <v>B</v>
       </c>
-      <c r="AL32" s="32"/>
-      <c r="AM32" s="32"/>
-      <c r="AO32" s="32"/>
-      <c r="AP32" s="32"/>
-      <c r="AR32" s="32"/>
-      <c r="AS32" s="32"/>
+      <c r="AL32" s="45"/>
+      <c r="AM32" s="45"/>
+      <c r="AO32" s="45"/>
+      <c r="AP32" s="45"/>
+      <c r="AR32" s="45"/>
+      <c r="AS32" s="45"/>
     </row>
     <row r="33" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="str">
@@ -25461,7 +25239,7 @@
         <f>+RawAfter!B34</f>
         <v>B</v>
       </c>
-      <c r="C34" s="48" t="str">
+      <c r="C34" s="38" t="str">
         <f>+RawAfter!C34</f>
         <v>B</v>
       </c>
@@ -25525,7 +25303,7 @@
         <f>+RawAfter!R34</f>
         <v>B</v>
       </c>
-      <c r="S34" s="48" t="str">
+      <c r="S34" s="38" t="str">
         <f>+RawAfter!S34</f>
         <v>B</v>
       </c>
@@ -25557,7 +25335,7 @@
         <f>+RawAfter!Z34</f>
         <v>B</v>
       </c>
-      <c r="AA34" s="48" t="str">
+      <c r="AA34" s="38" t="str">
         <f>+RawAfter!AA34</f>
         <v>B</v>
       </c>
@@ -26085,31 +25863,31 @@
         <f>+RawBefore!AJ1</f>
         <v>R</v>
       </c>
-      <c r="AK1" s="38" t="s">
+      <c r="AK1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AL1" s="38" t="s">
+      <c r="AL1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="38" t="s">
+      <c r="AM1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AN1" s="38" t="s">
+      <c r="AN1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AO1" s="38" t="s">
+      <c r="AO1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AP1" s="38" t="s">
+      <c r="AP1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AQ1" s="38" t="s">
+      <c r="AQ1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="38" t="s">
+      <c r="AR1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AS1" s="38" t="s">
+      <c r="AS1" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -26586,31 +26364,31 @@
         <f>+RawBefore!AJ4</f>
         <v>B</v>
       </c>
-      <c r="AK4" s="38" t="s">
+      <c r="AK4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AL4" s="38" t="s">
+      <c r="AL4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AM4" s="38" t="s">
+      <c r="AM4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AN4" s="38" t="s">
+      <c r="AN4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AO4" s="38" t="s">
+      <c r="AO4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AP4" s="38" t="s">
+      <c r="AP4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AQ4" s="38" t="s">
+      <c r="AQ4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AR4" s="38" t="s">
+      <c r="AR4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AS4" s="38" t="s">
+      <c r="AS4" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -27087,31 +26865,31 @@
         <f>+RawBefore!AJ7</f>
         <v>R</v>
       </c>
-      <c r="AK7" s="38" t="s">
+      <c r="AK7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AL7" s="38" t="s">
+      <c r="AL7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AM7" s="38" t="s">
+      <c r="AM7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AN7" s="38" t="s">
+      <c r="AN7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AO7" s="38" t="s">
+      <c r="AO7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AP7" s="38" t="s">
+      <c r="AP7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AQ7" s="38" t="s">
+      <c r="AQ7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AR7" s="38" t="s">
+      <c r="AR7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AS7" s="38" t="s">
+      <c r="AS7" s="34" t="s">
         <v>8</v>
       </c>
     </row>
@@ -27261,39 +27039,39 @@
         <v>B</v>
       </c>
       <c r="AK8" s="26">
-        <f>+AK2+AK5</f>
+        <f t="shared" ref="AK8:AS8" si="0">+AK2+AK5</f>
         <v>144</v>
       </c>
       <c r="AL8" s="26">
-        <f>+AL2+AL5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AM8" s="26">
-        <f>+AM2+AM5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AN8" s="26">
-        <f>+AN2+AN5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AO8" s="26">
-        <f>+AO2+AO5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AP8" s="26">
-        <f>+AP2+AP5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AQ8" s="26">
-        <f>+AQ2+AQ5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AR8" s="26">
-        <f>+AR2+AR5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AS8" s="26">
-        <f>+AS2+AS5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AT8" s="26"/>
@@ -27735,7 +27513,7 @@
         <f>+RawBefore!AJ11</f>
         <v>R</v>
       </c>
-      <c r="AT11" s="36"/>
+      <c r="AT11" s="32"/>
     </row>
     <row r="12" spans="1:46" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="str">
@@ -28320,31 +28098,31 @@
         <f>+RawBefore!AJ15</f>
         <v>R</v>
       </c>
-      <c r="AK15" s="38" t="s">
+      <c r="AK15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AL15" s="38" t="s">
+      <c r="AL15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AM15" s="38" t="s">
+      <c r="AM15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AN15" s="38" t="s">
+      <c r="AN15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AO15" s="38" t="s">
+      <c r="AO15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AP15" s="38" t="s">
+      <c r="AP15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AQ15" s="38" t="s">
+      <c r="AQ15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AR15" s="38" t="s">
+      <c r="AR15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AS15" s="38" t="s">
+      <c r="AS15" s="34" t="s">
         <v>10</v>
       </c>
     </row>
@@ -28493,40 +28271,40 @@
         <f>+RawBefore!AJ16</f>
         <v>B</v>
       </c>
-      <c r="AK16" s="37">
-        <f>+AK2/AK8</f>
+      <c r="AK16" s="33">
+        <f t="shared" ref="AK16:AS16" si="1">+AK2/AK8</f>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AL16" s="37">
-        <f>+AL2/AL8</f>
+      <c r="AL16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AM16" s="37">
-        <f>+AM2/AM8</f>
+      <c r="AM16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AN16" s="37">
-        <f>+AN2/AN8</f>
+      <c r="AN16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AO16" s="37">
-        <f>+AO2/AO8</f>
+      <c r="AO16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AP16" s="37">
-        <f>+AP2/AP8</f>
+      <c r="AP16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AQ16" s="37">
-        <f>+AQ2/AQ8</f>
+      <c r="AQ16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AR16" s="37">
-        <f>+AR2/AR8</f>
+      <c r="AR16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
-      <c r="AS16" s="37">
-        <f>+AS2/AS8</f>
+      <c r="AS16" s="33">
+        <f t="shared" si="1"/>
         <v>0.54861111111111116</v>
       </c>
     </row>
@@ -28675,40 +28453,40 @@
         <f>+RawBefore!AJ17</f>
         <v>R</v>
       </c>
-      <c r="AK17" s="43" t="str">
+      <c r="AK17" s="47" t="str">
         <f>IF(AK16&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AL17" s="44" t="str">
+      <c r="AL17" s="46" t="str">
         <f>IF(AL16&gt;0.5, "R","B")</f>
         <v>R</v>
       </c>
-      <c r="AM17" s="44" t="str">
-        <f t="shared" ref="AM17:AS17" si="0">IF(AM16&gt;0.5, "R","B")</f>
-        <v>R</v>
-      </c>
-      <c r="AN17" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>R</v>
-      </c>
-      <c r="AO17" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>R</v>
-      </c>
-      <c r="AP17" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>R</v>
-      </c>
-      <c r="AQ17" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>R</v>
-      </c>
-      <c r="AR17" s="44" t="str">
-        <f t="shared" si="0"/>
-        <v>R</v>
-      </c>
-      <c r="AS17" s="44" t="str">
-        <f t="shared" si="0"/>
+      <c r="AM17" s="46" t="str">
+        <f t="shared" ref="AM17:AS17" si="2">IF(AM16&gt;0.5, "R","B")</f>
+        <v>R</v>
+      </c>
+      <c r="AN17" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>R</v>
+      </c>
+      <c r="AO17" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>R</v>
+      </c>
+      <c r="AP17" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>R</v>
+      </c>
+      <c r="AQ17" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>R</v>
+      </c>
+      <c r="AR17" s="46" t="str">
+        <f t="shared" si="2"/>
+        <v>R</v>
+      </c>
+      <c r="AS17" s="46" t="str">
+        <f t="shared" si="2"/>
         <v>R</v>
       </c>
     </row>
@@ -28857,15 +28635,15 @@
         <f>+RawBefore!AJ18</f>
         <v>B</v>
       </c>
-      <c r="AK18" s="43"/>
-      <c r="AL18" s="44"/>
-      <c r="AM18" s="44"/>
-      <c r="AN18" s="44"/>
-      <c r="AO18" s="44"/>
-      <c r="AP18" s="44"/>
-      <c r="AQ18" s="44"/>
-      <c r="AR18" s="44"/>
-      <c r="AS18" s="44"/>
+      <c r="AK18" s="47"/>
+      <c r="AL18" s="46"/>
+      <c r="AM18" s="46"/>
+      <c r="AN18" s="46"/>
+      <c r="AO18" s="46"/>
+      <c r="AP18" s="46"/>
+      <c r="AQ18" s="46"/>
+      <c r="AR18" s="46"/>
+      <c r="AS18" s="46"/>
     </row>
     <row r="19" spans="1:45" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="str">
@@ -31698,31 +31476,31 @@
         <f>+RawAfter!AJ1</f>
         <v>R</v>
       </c>
-      <c r="AK1" s="38" t="s">
+      <c r="AK1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AL1" s="38" t="s">
+      <c r="AL1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="38" t="s">
+      <c r="AM1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AN1" s="38" t="s">
+      <c r="AN1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AO1" s="38" t="s">
+      <c r="AO1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AP1" s="38" t="s">
+      <c r="AP1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AQ1" s="38" t="s">
+      <c r="AQ1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="38" t="s">
+      <c r="AR1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="AS1" s="38" t="s">
+      <c r="AS1" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -31739,7 +31517,7 @@
         <f>+RawAfter!C2</f>
         <v>R</v>
       </c>
-      <c r="D2" s="47" t="str">
+      <c r="D2" s="37" t="str">
         <f>+RawAfter!D2</f>
         <v>B</v>
       </c>
@@ -32199,31 +31977,31 @@
         <f>+RawAfter!AJ4</f>
         <v>B</v>
       </c>
-      <c r="AK4" s="38" t="s">
+      <c r="AK4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AL4" s="38" t="s">
+      <c r="AL4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AM4" s="38" t="s">
+      <c r="AM4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AN4" s="38" t="s">
+      <c r="AN4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AO4" s="38" t="s">
+      <c r="AO4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AP4" s="38" t="s">
+      <c r="AP4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AQ4" s="38" t="s">
+      <c r="AQ4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AR4" s="38" t="s">
+      <c r="AR4" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="AS4" s="38" t="s">
+      <c r="AS4" s="34" t="s">
         <v>7</v>
       </c>
     </row>
@@ -32700,31 +32478,31 @@
         <f>+RawAfter!AJ7</f>
         <v>R</v>
       </c>
-      <c r="AK7" s="38" t="s">
+      <c r="AK7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AL7" s="38" t="s">
+      <c r="AL7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AM7" s="38" t="s">
+      <c r="AM7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AN7" s="38" t="s">
+      <c r="AN7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AO7" s="38" t="s">
+      <c r="AO7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AP7" s="38" t="s">
+      <c r="AP7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AQ7" s="38" t="s">
+      <c r="AQ7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AR7" s="38" t="s">
+      <c r="AR7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="AS7" s="38" t="s">
+      <c r="AS7" s="34" t="s">
         <v>8</v>
       </c>
     </row>
@@ -32874,39 +32652,39 @@
         <v>B</v>
       </c>
       <c r="AK8" s="26">
-        <f>+AK2+AK5</f>
+        <f t="shared" ref="AK8:AS8" si="0">+AK2+AK5</f>
         <v>144</v>
       </c>
       <c r="AL8" s="26">
-        <f>+AL2+AL5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AM8" s="26">
-        <f>+AM2+AM5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AN8" s="26">
-        <f>+AN2+AN5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AO8" s="26">
-        <f>+AO2+AO5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AP8" s="26">
-        <f>+AP2+AP5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AQ8" s="26">
-        <f>+AQ2+AQ5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AR8" s="26">
-        <f>+AR2+AR5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="AS8" s="26">
-        <f>+AS2+AS5</f>
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
     </row>
@@ -33201,31 +32979,31 @@
         <f>+RawAfter!AJ10</f>
         <v>B</v>
       </c>
-      <c r="AK10" s="54" t="s">
+      <c r="AK10" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="AL10" s="55" t="s">
+      <c r="AL10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AM10" s="55" t="s">
+      <c r="AM10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AN10" s="55" t="s">
+      <c r="AN10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AO10" s="55" t="s">
+      <c r="AO10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AP10" s="55" t="s">
+      <c r="AP10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AQ10" s="55" t="s">
+      <c r="AQ10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AR10" s="55" t="s">
+      <c r="AR10" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="AS10" s="55" t="s">
+      <c r="AS10" s="48" t="s">
         <v>28</v>
       </c>
     </row>
@@ -33374,15 +33152,15 @@
         <f>+RawAfter!AJ11</f>
         <v>R</v>
       </c>
-      <c r="AK11" s="54"/>
-      <c r="AL11" s="55"/>
-      <c r="AM11" s="55"/>
-      <c r="AN11" s="55"/>
-      <c r="AO11" s="55"/>
-      <c r="AP11" s="55"/>
-      <c r="AQ11" s="55"/>
-      <c r="AR11" s="55"/>
-      <c r="AS11" s="55"/>
+      <c r="AK11" s="50"/>
+      <c r="AL11" s="48"/>
+      <c r="AM11" s="48"/>
+      <c r="AN11" s="48"/>
+      <c r="AO11" s="48"/>
+      <c r="AP11" s="48"/>
+      <c r="AQ11" s="48"/>
+      <c r="AR11" s="48"/>
+      <c r="AS11" s="48"/>
     </row>
     <row r="12" spans="1:45" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="str">
@@ -33711,40 +33489,40 @@
         <f>+RawAfter!AJ13</f>
         <v>R</v>
       </c>
-      <c r="AK13" s="30">
+      <c r="AK13" s="28">
         <f>AK12/AK8</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AL13" s="30">
-        <f t="shared" ref="AL13:AS13" si="0">AL12/AL8</f>
+      <c r="AL13" s="28">
+        <f t="shared" ref="AL13:AS13" si="1">AL12/AL8</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AM13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AM13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AN13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AN13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AO13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AO13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AP13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AP13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AQ13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AQ13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AR13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AR13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="AS13" s="30">
-        <f t="shared" si="0"/>
+      <c r="AS13" s="28">
+        <f t="shared" si="1"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
@@ -34039,31 +33817,31 @@
         <f>+RawAfter!AJ15</f>
         <v>R</v>
       </c>
-      <c r="AK15" s="38" t="s">
+      <c r="AK15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AL15" s="38" t="s">
+      <c r="AL15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AM15" s="38" t="s">
+      <c r="AM15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AN15" s="38" t="s">
+      <c r="AN15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AO15" s="38" t="s">
+      <c r="AO15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AP15" s="38" t="s">
+      <c r="AP15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AQ15" s="38" t="s">
+      <c r="AQ15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AR15" s="38" t="s">
+      <c r="AR15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AS15" s="38" t="s">
+      <c r="AS15" s="34" t="s">
         <v>10</v>
       </c>
     </row>
@@ -34212,40 +33990,40 @@
         <f>+RawAfter!AJ16</f>
         <v>B</v>
       </c>
-      <c r="AK16" s="37">
-        <f>+AK2/AK8</f>
+      <c r="AK16" s="33">
+        <f t="shared" ref="AK16:AS16" si="2">+AK2/AK8</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AL16" s="37">
-        <f>+AL2/AL8</f>
+      <c r="AL16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AM16" s="37">
-        <f>+AM2/AM8</f>
+      <c r="AM16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AN16" s="37">
-        <f>+AN2/AN8</f>
+      <c r="AN16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AO16" s="37">
-        <f>+AO2/AO8</f>
+      <c r="AO16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AP16" s="37">
-        <f>+AP2/AP8</f>
+      <c r="AP16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AQ16" s="37">
-        <f>+AQ2/AQ8</f>
+      <c r="AQ16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AR16" s="37">
-        <f>+AR2/AR8</f>
+      <c r="AR16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AS16" s="37">
-        <f>+AS2/AS8</f>
+      <c r="AS16" s="33">
+        <f t="shared" si="2"/>
         <v>0.49305555555555558</v>
       </c>
     </row>
@@ -34394,40 +34172,40 @@
         <f>+RawAfter!AJ17</f>
         <v>B</v>
       </c>
-      <c r="AK17" s="45" t="str">
+      <c r="AK17" s="51" t="str">
         <f>IF(AK16&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AL17" s="46" t="str">
+      <c r="AL17" s="49" t="str">
         <f>IF(AL16&gt;0.5, "R","B")</f>
         <v>B</v>
       </c>
-      <c r="AM17" s="46" t="str">
-        <f t="shared" ref="AM17:AS17" si="1">IF(AM16&gt;0.5, "R","B")</f>
-        <v>B</v>
-      </c>
-      <c r="AN17" s="46" t="str">
-        <f t="shared" si="1"/>
-        <v>B</v>
-      </c>
-      <c r="AO17" s="46" t="str">
-        <f t="shared" si="1"/>
-        <v>B</v>
-      </c>
-      <c r="AP17" s="46" t="str">
-        <f t="shared" si="1"/>
-        <v>B</v>
-      </c>
-      <c r="AQ17" s="46" t="str">
-        <f t="shared" si="1"/>
-        <v>B</v>
-      </c>
-      <c r="AR17" s="46" t="str">
-        <f t="shared" si="1"/>
-        <v>B</v>
-      </c>
-      <c r="AS17" s="46" t="str">
-        <f t="shared" si="1"/>
+      <c r="AM17" s="49" t="str">
+        <f t="shared" ref="AM17:AS17" si="3">IF(AM16&gt;0.5, "R","B")</f>
+        <v>B</v>
+      </c>
+      <c r="AN17" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="AO17" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="AP17" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="AQ17" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="AR17" s="49" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+      <c r="AS17" s="49" t="str">
+        <f t="shared" si="3"/>
         <v>B</v>
       </c>
     </row>
@@ -34576,15 +34354,15 @@
         <f>+RawAfter!AJ18</f>
         <v>B</v>
       </c>
-      <c r="AK18" s="45"/>
-      <c r="AL18" s="46"/>
-      <c r="AM18" s="46"/>
-      <c r="AN18" s="46"/>
-      <c r="AO18" s="46"/>
-      <c r="AP18" s="46"/>
-      <c r="AQ18" s="46"/>
-      <c r="AR18" s="46"/>
-      <c r="AS18" s="46"/>
+      <c r="AK18" s="51"/>
+      <c r="AL18" s="49"/>
+      <c r="AM18" s="49"/>
+      <c r="AN18" s="49"/>
+      <c r="AO18" s="49"/>
+      <c r="AP18" s="49"/>
+      <c r="AQ18" s="49"/>
+      <c r="AR18" s="49"/>
+      <c r="AS18" s="49"/>
     </row>
     <row r="19" spans="1:45" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="str">
@@ -37378,51 +37156,51 @@
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A45" s="27">
+      <c r="A45" s="53">
         <f>+A39+A42</f>
         <v>144</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="E45" s="27">
+      <c r="B45" s="53"/>
+      <c r="E45" s="53">
         <f>+E39+E42</f>
         <v>144</v>
       </c>
-      <c r="F45" s="27"/>
-      <c r="I45" s="27">
+      <c r="F45" s="53"/>
+      <c r="I45" s="53">
         <f>+I39+I42</f>
         <v>144</v>
       </c>
-      <c r="J45" s="27"/>
-      <c r="M45" s="27">
+      <c r="J45" s="53"/>
+      <c r="M45" s="53">
         <f>+M39+M42</f>
         <v>144</v>
       </c>
-      <c r="N45" s="27"/>
-      <c r="Q45" s="27">
+      <c r="N45" s="53"/>
+      <c r="Q45" s="53">
         <f>+Q39+Q42</f>
         <v>144</v>
       </c>
-      <c r="R45" s="27"/>
-      <c r="U45" s="27">
+      <c r="R45" s="53"/>
+      <c r="U45" s="53">
         <f>+U39+U42</f>
         <v>144</v>
       </c>
-      <c r="V45" s="27"/>
-      <c r="Y45" s="27">
+      <c r="V45" s="53"/>
+      <c r="Y45" s="53">
         <f>+Y39+Y42</f>
         <v>144</v>
       </c>
-      <c r="Z45" s="27"/>
-      <c r="AC45" s="27">
+      <c r="Z45" s="53"/>
+      <c r="AC45" s="53">
         <f>+AC39+AC42</f>
         <v>144</v>
       </c>
-      <c r="AD45" s="27"/>
-      <c r="AG45" s="27">
+      <c r="AD45" s="53"/>
+      <c r="AG45" s="53">
         <f>+AG39+AG42</f>
         <v>144</v>
       </c>
-      <c r="AH45" s="27"/>
+      <c r="AH45" s="53"/>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -37497,83 +37275,55 @@
       </c>
     </row>
     <row r="51" spans="1:34" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28">
+      <c r="A51" s="52">
         <f>+A39/A45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="E51" s="28">
+      <c r="B51" s="52"/>
+      <c r="E51" s="52">
         <f>+E39/E45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="F51" s="28"/>
-      <c r="I51" s="28">
+      <c r="F51" s="52"/>
+      <c r="I51" s="52">
         <f>+I39/I45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="J51" s="28"/>
-      <c r="M51" s="28">
+      <c r="J51" s="52"/>
+      <c r="M51" s="52">
         <f>+M39/M45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="N51" s="28"/>
-      <c r="Q51" s="28">
+      <c r="N51" s="52"/>
+      <c r="Q51" s="52">
         <f>+Q39/Q45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="R51" s="28"/>
-      <c r="U51" s="28">
+      <c r="R51" s="52"/>
+      <c r="U51" s="52">
         <f>+U39/U45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="V51" s="28"/>
-      <c r="Y51" s="28">
+      <c r="V51" s="52"/>
+      <c r="Y51" s="52">
         <f>+Y39/Y45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="Z51" s="28"/>
-      <c r="AC51" s="28">
+      <c r="Z51" s="52"/>
+      <c r="AC51" s="52">
         <f>+AC39/AC45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AD51" s="28"/>
-      <c r="AG51" s="28">
+      <c r="AD51" s="52"/>
+      <c r="AG51" s="52">
         <f>+AG39/AG45</f>
         <v>0.49305555555555558</v>
       </c>
-      <c r="AH51" s="28"/>
+      <c r="AH51" s="52"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="36">
-    <mergeCell ref="AP10:AP11"/>
-    <mergeCell ref="AQ10:AQ11"/>
-    <mergeCell ref="AQ17:AQ18"/>
-    <mergeCell ref="AR17:AR18"/>
-    <mergeCell ref="AS17:AS18"/>
-    <mergeCell ref="AR10:AR11"/>
-    <mergeCell ref="AS10:AS11"/>
-    <mergeCell ref="AK10:AK11"/>
-    <mergeCell ref="AL10:AL11"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="AN10:AN11"/>
-    <mergeCell ref="AO10:AO11"/>
-    <mergeCell ref="AK17:AK18"/>
-    <mergeCell ref="AL17:AL18"/>
-    <mergeCell ref="AM17:AM18"/>
-    <mergeCell ref="AN17:AN18"/>
-    <mergeCell ref="AO17:AO18"/>
-    <mergeCell ref="AP17:AP18"/>
-    <mergeCell ref="AC51:AD51"/>
-    <mergeCell ref="AG51:AH51"/>
-    <mergeCell ref="Y45:Z45"/>
-    <mergeCell ref="AC45:AD45"/>
-    <mergeCell ref="AG45:AH45"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="Q51:R51"/>
     <mergeCell ref="U51:V51"/>
     <mergeCell ref="Y51:Z51"/>
     <mergeCell ref="A45:B45"/>
@@ -37582,6 +37332,34 @@
     <mergeCell ref="M45:N45"/>
     <mergeCell ref="Q45:R45"/>
     <mergeCell ref="U45:V45"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="AC51:AD51"/>
+    <mergeCell ref="AG51:AH51"/>
+    <mergeCell ref="Y45:Z45"/>
+    <mergeCell ref="AC45:AD45"/>
+    <mergeCell ref="AG45:AH45"/>
+    <mergeCell ref="AK17:AK18"/>
+    <mergeCell ref="AL17:AL18"/>
+    <mergeCell ref="AM17:AM18"/>
+    <mergeCell ref="AN17:AN18"/>
+    <mergeCell ref="AO17:AO18"/>
+    <mergeCell ref="AK10:AK11"/>
+    <mergeCell ref="AL10:AL11"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="AN10:AN11"/>
+    <mergeCell ref="AO10:AO11"/>
+    <mergeCell ref="AP10:AP11"/>
+    <mergeCell ref="AQ10:AQ11"/>
+    <mergeCell ref="AQ17:AQ18"/>
+    <mergeCell ref="AR17:AR18"/>
+    <mergeCell ref="AS17:AS18"/>
+    <mergeCell ref="AR10:AR11"/>
+    <mergeCell ref="AS10:AS11"/>
+    <mergeCell ref="AP17:AP18"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:AJ36">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
@@ -37602,83 +37380,83 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="H2" s="39" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="H2" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="34"/>
+      <c r="H3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -37697,7 +37475,7 @@
       <c r="D4">
         <v>144</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="29">
         <f t="shared" ref="E4:E12" si="0">IF(B4&gt;C4,1,0)</f>
         <v>1</v>
       </c>
@@ -37719,7 +37497,7 @@
       <c r="K4">
         <v>144</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="29">
         <v>1</v>
       </c>
       <c r="M4">
@@ -37741,7 +37519,7 @@
       <c r="D5">
         <v>144</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -37766,7 +37544,7 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="30">
         <v>1</v>
       </c>
     </row>
@@ -37785,7 +37563,7 @@
       <c r="D6">
         <v>144</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -37810,7 +37588,7 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6" s="34">
+      <c r="M6" s="30">
         <v>1</v>
       </c>
     </row>
@@ -37829,7 +37607,7 @@
       <c r="D7">
         <v>144</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -37851,7 +37629,7 @@
       <c r="K7">
         <v>144</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="29">
         <v>1</v>
       </c>
       <c r="M7">
@@ -37873,7 +37651,7 @@
       <c r="D8">
         <v>144</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -37898,7 +37676,7 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8" s="34">
+      <c r="M8" s="30">
         <v>1</v>
       </c>
     </row>
@@ -37917,7 +37695,7 @@
       <c r="D9">
         <v>144</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -37942,7 +37720,7 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9" s="34">
+      <c r="M9" s="30">
         <v>1</v>
       </c>
     </row>
@@ -37965,7 +37743,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -37983,7 +37761,7 @@
       <c r="K10">
         <v>144</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="29">
         <v>1</v>
       </c>
       <c r="M10">
@@ -38009,7 +37787,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -38030,7 +37808,7 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" s="34">
+      <c r="M11" s="30">
         <v>1</v>
       </c>
     </row>
@@ -38053,7 +37831,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="34">
+      <c r="F12" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -38074,7 +37852,7 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="30">
         <v>1</v>
       </c>
     </row>
@@ -38118,11 +37896,11 @@
         <f>+B14+C14</f>
         <v>1296</v>
       </c>
-      <c r="E14" s="41">
+      <c r="E14" s="35">
         <f>SUM(E4:E12)</f>
         <v>6</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="36">
         <f>SUM(F4:F12)</f>
         <v>3</v>
       </c>
@@ -38141,86 +37919,86 @@
         <f>+I14+J14</f>
         <v>1296</v>
       </c>
-      <c r="L14" s="41">
+      <c r="L14" s="35">
         <f>SUM(L4:L12)</f>
         <v>3</v>
       </c>
-      <c r="M14" s="42">
+      <c r="M14" s="36">
         <f>SUM(M4:M12)</f>
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="H17" s="39" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="H17" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="55"/>
+      <c r="M17" s="55"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38" t="s">
+      <c r="G18" s="34"/>
+      <c r="H18" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="38" t="s">
+      <c r="I18" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="38" t="s">
+      <c r="J18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="K18" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="38" t="s">
+      <c r="L18" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="38" t="s">
+      <c r="M18" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -38239,7 +38017,7 @@
       <c r="D19">
         <v>144</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="29">
         <f t="shared" ref="E19:E27" si="2">IF(B19&gt;C19,1,0)</f>
         <v>1</v>
       </c>
@@ -38265,7 +38043,7 @@
         <f t="shared" ref="L19:L27" si="4">IF(I19&gt;J19,1,0)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="34">
+      <c r="M19" s="30">
         <f t="shared" ref="M19:M27" si="5">IF(I19&lt;J19,1,0)</f>
         <v>1</v>
       </c>
@@ -38285,7 +38063,7 @@
       <c r="D20">
         <v>144</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38311,7 +38089,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M20" s="34">
+      <c r="M20" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38331,7 +38109,7 @@
       <c r="D21">
         <v>144</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38357,7 +38135,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38377,7 +38155,7 @@
       <c r="D22">
         <v>144</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38403,7 +38181,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M22" s="34">
+      <c r="M22" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38423,7 +38201,7 @@
       <c r="D23">
         <v>144</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38449,7 +38227,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M23" s="34">
+      <c r="M23" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38469,7 +38247,7 @@
       <c r="D24">
         <v>144</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38495,7 +38273,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M24" s="34">
+      <c r="M24" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38515,7 +38293,7 @@
       <c r="D25">
         <v>144</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38541,7 +38319,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M25" s="34">
+      <c r="M25" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38561,7 +38339,7 @@
       <c r="D26">
         <v>144</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38587,7 +38365,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M26" s="34">
+      <c r="M26" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38607,7 +38385,7 @@
       <c r="D27">
         <v>144</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="29">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -38633,7 +38411,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M27" s="34">
+      <c r="M27" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
@@ -38678,11 +38456,11 @@
         <f>SUM(D19:D27)</f>
         <v>1296</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="35">
         <f>SUM(E19:E27)</f>
         <v>9</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="36">
         <f>SUM(F19:F27)</f>
         <v>0</v>
       </c>
@@ -38701,11 +38479,11 @@
         <f>SUM(K19:K27)</f>
         <v>1296</v>
       </c>
-      <c r="L29" s="41">
+      <c r="L29" s="35">
         <f>SUM(L19:L27)</f>
         <v>0</v>
       </c>
-      <c r="M29" s="42">
+      <c r="M29" s="36">
         <f>SUM(M19:M27)</f>
         <v>9</v>
       </c>

</xml_diff>